<commit_message>
Mas Practica Mi hermano, menos teoria
</commit_message>
<xml_diff>
--- a/IdeasPracticas.xlsx
+++ b/IdeasPracticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5FE84-E627-4805-9BE5-9D9915028535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50FCC7-A864-4387-8BAC-26CB4F6DA702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>IDEAS</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>INTERACTUAR ENTRE ARCHIVOS EN C</t>
+  </si>
+  <si>
+    <t>PRACTICA Y PRACTICA, MUCHA PRACTICA. 10/09/2024</t>
+  </si>
+  <si>
+    <t>PRACTICA Y PRACTICA, MUCHA MAS. 10/09/2024</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,6 +453,16 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" location="cc" display="https://github.com/practical-tutorials/project-based-learning - cc" xr:uid="{69F99468-2798-43B8-B452-6E4DA40DA676}"/>

</xml_diff>